<commit_message>
Fixed a bug processing None cov_nev when interpolating a survey.
</commit_message>
<xml_diff>
--- a/tests/test_data/error_mwdrev5_iscwsa_validation_results.xlsx
+++ b/tests/test_data/error_mwdrev5_iscwsa_validation_results.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -3179,7 +3179,7 @@
         <v>-0.0186</v>
       </c>
       <c r="J41" t="n">
-        <v>0.8922731146735273</v>
+        <v>0.8922731146735275</v>
       </c>
       <c r="K41" t="n">
         <v>0.02014056202278082</v>
@@ -3316,19 +3316,19 @@
         <v>0.1212776876267033</v>
       </c>
       <c r="K43" t="n">
-        <v>0.001825519292217056</v>
+        <v>0.001825519292217054</v>
       </c>
       <c r="L43" t="n">
         <v>0.01159560265567282</v>
       </c>
       <c r="M43" t="n">
-        <v>0.01487933998798403</v>
+        <v>0.01487933998798402</v>
       </c>
       <c r="N43" t="n">
         <v>-0.03750050501950686</v>
       </c>
       <c r="O43" t="n">
-        <v>-0.004600869086685043</v>
+        <v>-0.00460086908668504</v>
       </c>
       <c r="P43" t="n">
         <v>-0</v>
@@ -3916,16 +3916,16 @@
         <v>0</v>
       </c>
       <c r="J52" t="n">
-        <v>0.1128319071378604</v>
+        <v>0.1128319071378605</v>
       </c>
       <c r="K52" t="n">
-        <v>0.008100966454352095</v>
+        <v>0.0081009664543521</v>
       </c>
       <c r="L52" t="n">
         <v>0</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.03023321839805313</v>
+        <v>-0.03023321839805315</v>
       </c>
       <c r="N52" t="n">
         <v>-0</v>
@@ -3986,13 +3986,13 @@
         <v>0.1229338594805348</v>
       </c>
       <c r="K53" t="n">
-        <v>0.00882625400046687</v>
+        <v>0.008826254000466872</v>
       </c>
       <c r="L53" t="n">
         <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>-0.03294002837025041</v>
+        <v>-0.03294002837025042</v>
       </c>
       <c r="N53" t="n">
         <v>0</v>
@@ -4050,10 +4050,10 @@
         <v>0</v>
       </c>
       <c r="J54" t="n">
-        <v>0.8474460279399308</v>
+        <v>0.8474460279399311</v>
       </c>
       <c r="K54" t="n">
-        <v>0.06084388732193766</v>
+        <v>0.06084388732193767</v>
       </c>
       <c r="L54" t="n">
         <v>0</v>
@@ -5594,19 +5594,19 @@
         <v>6.604970767711233</v>
       </c>
       <c r="K77" t="n">
-        <v>0.0005334286404197735</v>
+        <v>0.0005334286404197724</v>
       </c>
       <c r="L77" t="n">
         <v>0.4372699718087822</v>
       </c>
       <c r="M77" t="n">
-        <v>0.05935722851205699</v>
+        <v>0.05935722851205692</v>
       </c>
       <c r="N77" t="n">
         <v>-1.69945737851672</v>
       </c>
       <c r="O77" t="n">
-        <v>-0.01527260051721223</v>
+        <v>-0.01527260051721222</v>
       </c>
       <c r="P77" t="n">
         <v>-0</v>
@@ -5728,19 +5728,19 @@
         <v>10.00801738186408</v>
       </c>
       <c r="K79" t="n">
-        <v>0.0265946168176742</v>
+        <v>0.02659461681767429</v>
       </c>
       <c r="L79" t="n">
         <v>1.051501499777051</v>
       </c>
       <c r="M79" t="n">
-        <v>-0.5159063746216926</v>
+        <v>-0.5159063746216935</v>
       </c>
       <c r="N79" t="n">
         <v>-3.243986018284431</v>
       </c>
       <c r="O79" t="n">
-        <v>0.1672252357444307</v>
+        <v>0.1672252357444309</v>
       </c>
       <c r="P79" t="n">
         <v>0</v>
@@ -5795,19 +5795,19 @@
         <v>2.059295270897338</v>
       </c>
       <c r="K80" t="n">
-        <v>0.003033129771511088</v>
+        <v>0.003033129771511093</v>
       </c>
       <c r="L80" t="n">
         <v>0.2148580231702464</v>
       </c>
       <c r="M80" t="n">
-        <v>-0.07903233385450988</v>
+        <v>-0.07903233385450993</v>
       </c>
       <c r="N80" t="n">
         <v>-0.6651737449936213</v>
       </c>
       <c r="O80" t="n">
-        <v>0.02552826407583746</v>
+        <v>0.02552826407583748</v>
       </c>
       <c r="P80" t="n">
         <v>-0</v>
@@ -5862,19 +5862,19 @@
         <v>1.029647635448671</v>
       </c>
       <c r="K81" t="n">
-        <v>0.001516564885755541</v>
+        <v>0.001516564885755545</v>
       </c>
       <c r="L81" t="n">
         <v>0.1074290115851228</v>
       </c>
       <c r="M81" t="n">
-        <v>-0.03951616692725494</v>
+        <v>-0.03951616692725499</v>
       </c>
       <c r="N81" t="n">
         <v>-0.3325868724968104</v>
       </c>
       <c r="O81" t="n">
-        <v>0.0127641320379187</v>
+        <v>0.01276413203791871</v>
       </c>
       <c r="P81" t="n">
         <v>0</v>
@@ -5996,19 +5996,19 @@
         <v>4.118590541794685</v>
       </c>
       <c r="K83" t="n">
-        <v>0.006066259543022165</v>
+        <v>0.006066259543022178</v>
       </c>
       <c r="L83" t="n">
         <v>0.4297160463404913</v>
       </c>
       <c r="M83" t="n">
-        <v>-0.1580646677090198</v>
+        <v>-0.1580646677090199</v>
       </c>
       <c r="N83" t="n">
         <v>-1.330347489987242</v>
       </c>
       <c r="O83" t="n">
-        <v>0.05105652815167479</v>
+        <v>0.05105652815167485</v>
       </c>
       <c r="P83" t="n">
         <v>-0</v>
@@ -6328,7 +6328,7 @@
         <v>0</v>
       </c>
       <c r="J88" t="n">
-        <v>6.21122716217903</v>
+        <v>6.211227162179044</v>
       </c>
       <c r="K88" t="n">
         <v>0.445946046269472</v>
@@ -6337,7 +6337,7 @@
         <v>0</v>
       </c>
       <c r="M88" t="n">
-        <v>-1.664293302112128</v>
+        <v>-1.66429330211213</v>
       </c>
       <c r="N88" t="n">
         <v>-0</v>
@@ -8006,19 +8006,19 @@
         <v>7.064622943012132</v>
       </c>
       <c r="K113" t="n">
-        <v>0.0001111710075633799</v>
+        <v>0.0001111710075633793</v>
       </c>
       <c r="L113" t="n">
         <v>0.4767211149502918</v>
       </c>
       <c r="M113" t="n">
-        <v>0.02802465433560295</v>
+        <v>0.02802465433560287</v>
       </c>
       <c r="N113" t="n">
         <v>-1.835171633961291</v>
       </c>
       <c r="O113" t="n">
-        <v>-0.00727994276596745</v>
+        <v>-0.007279942765967429</v>
       </c>
       <c r="P113" t="n">
         <v>0</v>
@@ -8140,19 +8140,19 @@
         <v>43.45344171508508</v>
       </c>
       <c r="K115" t="n">
-        <v>1.105639477520931</v>
+        <v>1.105639477520932</v>
       </c>
       <c r="L115" t="n">
         <v>4.829740109873929</v>
       </c>
       <c r="M115" t="n">
-        <v>-6.931366430535388</v>
+        <v>-6.931366430535392</v>
       </c>
       <c r="N115" t="n">
         <v>-14.48685025681619</v>
       </c>
       <c r="O115" t="n">
-        <v>2.310833471205334</v>
+        <v>2.310833471205335</v>
       </c>
       <c r="P115" t="n">
         <v>0</v>
@@ -8207,19 +8207,19 @@
         <v>2.2685541829693</v>
       </c>
       <c r="K116" t="n">
-        <v>0.004273186169655878</v>
+        <v>0.004273186169655883</v>
       </c>
       <c r="L116" t="n">
         <v>0.237322240904163</v>
       </c>
       <c r="M116" t="n">
-        <v>-0.09845788114609923</v>
+        <v>-0.09845788114609928</v>
       </c>
       <c r="N116" t="n">
         <v>-0.7337427085258066</v>
       </c>
       <c r="O116" t="n">
-        <v>0.03184528407132538</v>
+        <v>0.0318452840713254</v>
       </c>
       <c r="P116" t="n">
         <v>-0</v>
@@ -8274,19 +8274,19 @@
         <v>1.134277091484652</v>
       </c>
       <c r="K117" t="n">
-        <v>0.002136593084827936</v>
+        <v>0.00213659308482794</v>
       </c>
       <c r="L117" t="n">
         <v>0.1186611204520811</v>
       </c>
       <c r="M117" t="n">
-        <v>-0.04922894057304963</v>
+        <v>-0.04922894057304968</v>
       </c>
       <c r="N117" t="n">
         <v>-0.3668713542629031</v>
       </c>
       <c r="O117" t="n">
-        <v>0.01592264203566265</v>
+        <v>0.01592264203566267</v>
       </c>
       <c r="P117" t="n">
         <v>-0</v>
@@ -8408,19 +8408,19 @@
         <v>4.537108365938608</v>
       </c>
       <c r="K119" t="n">
-        <v>0.008546372339311744</v>
+        <v>0.008546372339311761</v>
       </c>
       <c r="L119" t="n">
         <v>0.4746444818083245</v>
       </c>
       <c r="M119" t="n">
-        <v>-0.1969157622921985</v>
+        <v>-0.1969157622921987</v>
       </c>
       <c r="N119" t="n">
         <v>-1.467485417051613</v>
       </c>
       <c r="O119" t="n">
-        <v>0.0636905681426506</v>
+        <v>0.06369056814265067</v>
       </c>
       <c r="P119" t="n">
         <v>0</v>
@@ -8740,7 +8740,7 @@
         <v>0</v>
       </c>
       <c r="J124" t="n">
-        <v>4.959636858094734</v>
+        <v>4.959636858094745</v>
       </c>
       <c r="K124" t="n">
         <v>0.3560859054177269</v>
@@ -8749,7 +8749,7 @@
         <v>0</v>
       </c>
       <c r="M124" t="n">
-        <v>-1.328930690878119</v>
+        <v>-1.32893069087812</v>
       </c>
       <c r="N124" t="n">
         <v>-0</v>
@@ -10184,6 +10184,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>